<commit_message>
made changes to xlsx file for plotting
</commit_message>
<xml_diff>
--- a/variable_noise_sim_real.xlsx
+++ b/variable_noise_sim_real.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0f4b32f1ebc25b5/Documents/GitHub/ECE303LAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B149F01-546E-41FC-9EEE-8A74AD2D9848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{9B149F01-546E-41FC-9EEE-8A74AD2D9848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B46776-9623-4905-96CE-7751F98006ED}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{14DA560B-23B4-4392-A5B2-7878BEED6803}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="21705" xr2:uid="{14DA560B-23B4-4392-A5B2-7878BEED6803}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,6 +110,1085 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Noise Testing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> With Variable Noise Magnitude</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.666717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.33253</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0001799999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6669100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3336299999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0002899999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3300400000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0004900000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6671800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.15136E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5355400000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2044700000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1174100000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05016E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.21761E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.40835E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5758000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7670900000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.91014E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F54A-42D3-902B-5E61F58D5D7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="911065376"/>
+        <c:axId val="911062976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="911065376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Collector Voltage (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="911062976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="911062976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Vout (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="911065376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE86D7C5-5FBE-CD8E-1996-ED1F66E7E262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,17 +1511,17 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -456,12 +1535,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.666717</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -470,12 +1546,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1.33253</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -484,12 +1557,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2.0001799999999998</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -498,12 +1568,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>2.6669100000000001</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -512,12 +1579,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>3.3336299999999999</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -526,12 +1590,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>4.0002899999999997</v>
+        <v>200</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -540,12 +1601,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>4.6669999999999998</v>
+        <v>500</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -554,12 +1612,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>5.3300400000000003</v>
+        <v>1000</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -568,12 +1623,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>6.0004900000000001</v>
+        <v>10000</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -582,12 +1634,9 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>6.6671800000000001</v>
+        <v>100000</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -596,12 +1645,12 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -615,9 +1664,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>0.666717</v>
       </c>
       <c r="B16" s="1">
         <v>2.15136E-6</v>
@@ -629,9 +1678,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2</v>
+        <v>1.33253</v>
       </c>
       <c r="B17" s="1">
         <v>4.5355400000000003E-6</v>
@@ -643,9 +1692,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>2.0001799999999998</v>
       </c>
       <c r="B18" s="1">
         <v>6.2044700000000001E-6</v>
@@ -657,9 +1706,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>2.6669100000000001</v>
       </c>
       <c r="B19" s="1">
         <v>8.1174100000000003E-6</v>
@@ -671,9 +1720,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5</v>
+        <v>3.3336299999999999</v>
       </c>
       <c r="B20" s="1">
         <v>1.05016E-5</v>
@@ -685,9 +1734,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6</v>
+        <v>4.0002899999999997</v>
       </c>
       <c r="B21" s="1">
         <v>1.21761E-5</v>
@@ -699,9 +1748,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7</v>
+        <v>4.6669999999999998</v>
       </c>
       <c r="B22" s="1">
         <v>1.40835E-5</v>
@@ -713,9 +1762,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8</v>
+        <v>5.3300400000000003</v>
       </c>
       <c r="B23" s="1">
         <v>1.5758000000000001E-5</v>
@@ -727,9 +1776,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>9</v>
+        <v>6.0004900000000001</v>
       </c>
       <c r="B24" s="1">
         <v>1.7670900000000001E-5</v>
@@ -741,9 +1790,9 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>10</v>
+        <v>6.6671800000000001</v>
       </c>
       <c r="B25" s="1">
         <v>1.91014E-5</v>
@@ -757,5 +1806,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>